<commit_message>
Refactor peak detection algorithm for improved accuracy
</commit_message>
<xml_diff>
--- a/data/benjamin_2_csv/Tableau récapitulatif - new algo.xlsx
+++ b/data/benjamin_2_csv/Tableau récapitulatif - new algo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abarb\Documents\travail\stage et4\travail\codePlateau\data\benjamin_2_csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F81341F-7727-424D-A899-A902356B6E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D9919E-D897-4134-9E86-0384DCA77C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5738" yWindow="3472" windowWidth="16200" windowHeight="8296" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
@@ -1074,19 +1074,19 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="6">
-        <v>428.96100000000001</v>
+        <v>450.863</v>
       </c>
       <c r="L3" s="6">
-        <v>407</v>
+        <v>425</v>
       </c>
       <c r="M3" s="6">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N3" s="6">
-        <v>145.55800000000013</v>
+        <v>154.74100000000013</v>
       </c>
       <c r="O3" s="6">
-        <v>4.8520000000000003</v>
+        <v>4.992</v>
       </c>
       <c r="P3" s="6">
         <v>11.913000000000011</v>
@@ -1095,10 +1095,10 @@
         <v>0.20200000000005502</v>
       </c>
       <c r="R3" s="6">
-        <v>33.9</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="S3" s="6">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T3" s="6" t="s">
         <v>33</v>

</xml_diff>